<commit_message>
Adding HTTP response saving and Testcase008
</commit_message>
<xml_diff>
--- a/webtesting/resources/InvalidLogin.xlsx
+++ b/webtesting/resources/InvalidLogin.xlsx
@@ -37,7 +37,7 @@
     <t>Aa123456</t>
   </si>
   <si>
-    <t>john210@test.com</t>
+    <t>john310@test.com</t>
   </si>
   <si>
     <t>01234567890</t>
@@ -46,13 +46,13 @@
     <t>John</t>
   </si>
   <si>
-    <t>john212@test.com</t>
+    <t>john312@test.com</t>
   </si>
   <si>
-    <t>john213@test.com</t>
+    <t>john313@test.com</t>
   </si>
   <si>
-    <t>john214@test.com</t>
+    <t>john314@test.com</t>
   </si>
   <si>
     <t>Invalid_FirstName</t>
@@ -61,7 +61,7 @@
     <t>john</t>
   </si>
   <si>
-    <t>john215@test.com</t>
+    <t>john315@test.com</t>
   </si>
   <si>
     <t>01234567891</t>
@@ -73,10 +73,10 @@
     <t>doe</t>
   </si>
   <si>
-    <t>john216@test.com</t>
+    <t>john316@test.com</t>
   </si>
   <si>
-    <t>john217@test.com</t>
+    <t>john317@test.com</t>
   </si>
   <si>
     <t>Invalid_Password</t>
@@ -85,58 +85,58 @@
     <t>aa123456</t>
   </si>
   <si>
-    <t>john218@test.com</t>
+    <t>john318@test.com</t>
   </si>
   <si>
     <t>AA123456</t>
   </si>
   <si>
-    <t>john219@test.com</t>
+    <t>john319@test.com</t>
   </si>
   <si>
     <t>12345678</t>
   </si>
   <si>
-    <t>john220@test.com</t>
+    <t>john320@test.com</t>
   </si>
   <si>
     <t>Aa12345</t>
   </si>
   <si>
-    <t>john221@test.com</t>
+    <t>john321@test.com</t>
   </si>
   <si>
     <t>Invalid_Email</t>
   </si>
   <si>
-    <t>john212@test</t>
+    <t>john312@test</t>
   </si>
   <si>
-    <t>john212@test.</t>
+    <t>john312@test.</t>
   </si>
   <si>
-    <t>john212@.com</t>
+    <t>john312@.com</t>
   </si>
   <si>
-    <t>john212.com</t>
+    <t>john312.com</t>
   </si>
   <si>
-    <t>john212@</t>
+    <t>john312@</t>
   </si>
   <si>
-    <t>john212</t>
+    <t>john312</t>
   </si>
   <si>
     <t>Invalid_Phone</t>
   </si>
   <si>
-    <t>john222@test.com</t>
+    <t>john322@test.com</t>
   </si>
   <si>
     <t>abcdefghijk</t>
   </si>
   <si>
-    <t>john223@test.com</t>
+    <t>john323@test.com</t>
   </si>
   <si>
     <t>1111</t>
@@ -145,14 +145,14 @@
     <t>Valid_Data</t>
   </si>
   <si>
-    <t>john224@test.com</t>
+    <t>john324@test.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="9">
+  <fonts count="7">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -181,13 +181,8 @@
       <name val="Arial"/>
     </font>
     <font>
-      <b/>
-      <name val="Arial"/>
-    </font>
-    <font/>
-    <font>
       <u/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF1155CC"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -217,7 +212,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="11">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -248,19 +243,7 @@
     <xf borderId="0" fillId="2" fontId="5" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="6" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -756,7 +739,7 @@
       <c r="AC7" s="4"/>
     </row>
     <row r="8">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -812,7 +795,7 @@
       <c r="E9" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="F9" s="6" t="s">
         <v>17</v>
       </c>
       <c r="G9" s="3"/>
@@ -846,7 +829,7 @@
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
-      <c r="G10" s="10" t="s">
+      <c r="G10" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H10" s="4"/>
@@ -873,7 +856,7 @@
       <c r="AC10" s="4"/>
     </row>
     <row r="11">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -891,7 +874,7 @@
       <c r="F11" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G11" s="11"/>
+      <c r="G11" s="3"/>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
@@ -916,23 +899,23 @@
       <c r="AC11" s="4"/>
     </row>
     <row r="12">
-      <c r="A12" s="12"/>
-      <c r="B12" s="13" t="s">
+      <c r="A12" s="5"/>
+      <c r="B12" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" s="6" t="s">
         <v>7</v>
       </c>
       <c r="E12" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="F12" s="7" t="s">
+      <c r="F12" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="G12" s="11"/>
+      <c r="G12" s="3"/>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
@@ -957,23 +940,23 @@
       <c r="AC12" s="4"/>
     </row>
     <row r="13">
-      <c r="A13" s="12"/>
-      <c r="B13" s="13" t="s">
+      <c r="A13" s="5"/>
+      <c r="B13" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="6" t="s">
         <v>7</v>
       </c>
       <c r="E13" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="F13" s="7" t="s">
+      <c r="F13" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="G13" s="11"/>
+      <c r="G13" s="3"/>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
@@ -998,13 +981,13 @@
       <c r="AC13" s="4"/>
     </row>
     <row r="14">
-      <c r="A14" s="12"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="10" t="s">
+      <c r="A14" s="5"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="1" t="s">
         <v>18</v>
       </c>
       <c r="H14" s="4"/>
@@ -1031,7 +1014,7 @@
       <c r="AC14" s="4"/>
     </row>
     <row r="15">
-      <c r="A15" s="10" t="s">
+      <c r="A15" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -1049,7 +1032,7 @@
       <c r="F15" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G15" s="11"/>
+      <c r="G15" s="3"/>
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
       <c r="J15" s="4"/>
@@ -1074,23 +1057,23 @@
       <c r="AC15" s="4"/>
     </row>
     <row r="16">
-      <c r="A16" s="12"/>
-      <c r="B16" s="7" t="s">
+      <c r="A16" s="5"/>
+      <c r="B16" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D16" s="6" t="s">
         <v>23</v>
       </c>
       <c r="E16" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F16" s="7" t="s">
+      <c r="F16" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="G16" s="11"/>
+      <c r="G16" s="3"/>
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
@@ -1115,23 +1098,23 @@
       <c r="AC16" s="4"/>
     </row>
     <row r="17">
-      <c r="A17" s="12"/>
-      <c r="B17" s="7" t="s">
+      <c r="A17" s="5"/>
+      <c r="B17" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C17" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="D17" s="6" t="s">
         <v>25</v>
       </c>
       <c r="E17" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="F17" s="7" t="s">
+      <c r="F17" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="G17" s="11"/>
+      <c r="G17" s="3"/>
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
       <c r="J17" s="4"/>
@@ -1156,23 +1139,23 @@
       <c r="AC17" s="4"/>
     </row>
     <row r="18">
-      <c r="A18" s="12"/>
-      <c r="B18" s="7" t="s">
+      <c r="A18" s="5"/>
+      <c r="B18" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="C18" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D18" s="7" t="s">
+      <c r="D18" s="6" t="s">
         <v>27</v>
       </c>
       <c r="E18" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="F18" s="7" t="s">
+      <c r="F18" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="G18" s="11"/>
+      <c r="G18" s="3"/>
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
       <c r="J18" s="4"/>
@@ -1197,23 +1180,23 @@
       <c r="AC18" s="4"/>
     </row>
     <row r="19">
-      <c r="A19" s="12"/>
-      <c r="B19" s="7" t="s">
+      <c r="A19" s="5"/>
+      <c r="B19" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C19" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="D19" s="6" t="s">
         <v>29</v>
       </c>
       <c r="E19" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F19" s="7" t="s">
+      <c r="F19" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="G19" s="11"/>
+      <c r="G19" s="3"/>
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
       <c r="J19" s="4"/>
@@ -1238,13 +1221,13 @@
       <c r="AC19" s="4"/>
     </row>
     <row r="20">
-      <c r="A20" s="12"/>
-      <c r="B20" s="12"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="10" t="s">
+      <c r="A20" s="5"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="1" t="s">
         <v>22</v>
       </c>
       <c r="H20" s="4"/>
@@ -1271,7 +1254,7 @@
       <c r="AC20" s="4"/>
     </row>
     <row r="21">
-      <c r="A21" s="10" t="s">
+      <c r="A21" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B21" s="2" t="s">
@@ -1289,7 +1272,7 @@
       <c r="F21" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G21" s="11"/>
+      <c r="G21" s="3"/>
       <c r="H21" s="4"/>
       <c r="I21" s="4"/>
       <c r="J21" s="4"/>
@@ -1314,23 +1297,23 @@
       <c r="AC21" s="4"/>
     </row>
     <row r="22">
-      <c r="A22" s="12"/>
-      <c r="B22" s="7" t="s">
+      <c r="A22" s="5"/>
+      <c r="B22" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="C22" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D22" s="7" t="s">
+      <c r="D22" s="6" t="s">
         <v>7</v>
       </c>
       <c r="E22" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="F22" s="7" t="s">
+      <c r="F22" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="G22" s="11"/>
+      <c r="G22" s="3"/>
       <c r="H22" s="4"/>
       <c r="I22" s="4"/>
       <c r="J22" s="4"/>
@@ -1355,23 +1338,23 @@
       <c r="AC22" s="4"/>
     </row>
     <row r="23">
-      <c r="A23" s="12"/>
-      <c r="B23" s="7" t="s">
+      <c r="A23" s="5"/>
+      <c r="B23" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="C23" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D23" s="7" t="s">
+      <c r="D23" s="6" t="s">
         <v>7</v>
       </c>
       <c r="E23" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="F23" s="7" t="s">
+      <c r="F23" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="G23" s="11"/>
+      <c r="G23" s="3"/>
       <c r="H23" s="4"/>
       <c r="I23" s="4"/>
       <c r="J23" s="4"/>
@@ -1396,23 +1379,23 @@
       <c r="AC23" s="4"/>
     </row>
     <row r="24">
-      <c r="A24" s="12"/>
-      <c r="B24" s="7" t="s">
+      <c r="A24" s="5"/>
+      <c r="B24" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C24" s="7" t="s">
+      <c r="C24" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D24" s="7" t="s">
+      <c r="D24" s="6" t="s">
         <v>7</v>
       </c>
       <c r="E24" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="F24" s="7" t="s">
+      <c r="F24" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="G24" s="11"/>
+      <c r="G24" s="3"/>
       <c r="H24" s="4"/>
       <c r="I24" s="4"/>
       <c r="J24" s="4"/>
@@ -1437,23 +1420,23 @@
       <c r="AC24" s="4"/>
     </row>
     <row r="25">
-      <c r="A25" s="12"/>
-      <c r="B25" s="7" t="s">
+      <c r="A25" s="5"/>
+      <c r="B25" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C25" s="7" t="s">
+      <c r="C25" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D25" s="7" t="s">
+      <c r="D25" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E25" s="14" t="s">
+      <c r="E25" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="F25" s="7" t="s">
+      <c r="F25" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="G25" s="11"/>
+      <c r="G25" s="3"/>
       <c r="H25" s="4"/>
       <c r="I25" s="4"/>
       <c r="J25" s="4"/>
@@ -1478,23 +1461,23 @@
       <c r="AC25" s="4"/>
     </row>
     <row r="26">
-      <c r="A26" s="12"/>
-      <c r="B26" s="7" t="s">
+      <c r="A26" s="5"/>
+      <c r="B26" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C26" s="7" t="s">
+      <c r="C26" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D26" s="7" t="s">
+      <c r="D26" s="6" t="s">
         <v>7</v>
       </c>
       <c r="E26" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="F26" s="7" t="s">
+      <c r="F26" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="G26" s="11"/>
+      <c r="G26" s="3"/>
       <c r="H26" s="4"/>
       <c r="I26" s="4"/>
       <c r="J26" s="4"/>
@@ -1519,23 +1502,23 @@
       <c r="AC26" s="4"/>
     </row>
     <row r="27">
-      <c r="A27" s="12"/>
-      <c r="B27" s="7" t="s">
+      <c r="A27" s="5"/>
+      <c r="B27" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C27" s="7" t="s">
+      <c r="C27" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D27" s="7" t="s">
+      <c r="D27" s="6" t="s">
         <v>7</v>
       </c>
       <c r="E27" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="F27" s="7" t="s">
+      <c r="F27" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="G27" s="11"/>
+      <c r="G27" s="3"/>
       <c r="H27" s="4"/>
       <c r="I27" s="4"/>
       <c r="J27" s="4"/>
@@ -1560,13 +1543,13 @@
       <c r="AC27" s="4"/>
     </row>
     <row r="28">
-      <c r="A28" s="12"/>
-      <c r="B28" s="12"/>
-      <c r="C28" s="12"/>
-      <c r="D28" s="12"/>
-      <c r="E28" s="12"/>
-      <c r="F28" s="12"/>
-      <c r="G28" s="10" t="s">
+      <c r="A28" s="5"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="1" t="s">
         <v>31</v>
       </c>
       <c r="H28" s="4"/>
@@ -1593,7 +1576,7 @@
       <c r="AC28" s="4"/>
     </row>
     <row r="29">
-      <c r="A29" s="10" t="s">
+      <c r="A29" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B29" s="2" t="s">
@@ -1611,7 +1594,7 @@
       <c r="F29" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G29" s="11"/>
+      <c r="G29" s="3"/>
       <c r="H29" s="4"/>
       <c r="I29" s="4"/>
       <c r="J29" s="4"/>
@@ -1636,23 +1619,23 @@
       <c r="AC29" s="4"/>
     </row>
     <row r="30">
-      <c r="A30" s="12"/>
-      <c r="B30" s="7" t="s">
+      <c r="A30" s="5"/>
+      <c r="B30" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C30" s="7" t="s">
+      <c r="C30" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D30" s="7" t="s">
+      <c r="D30" s="6" t="s">
         <v>7</v>
       </c>
       <c r="E30" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="F30" s="7" t="s">
+      <c r="F30" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="G30" s="11"/>
+      <c r="G30" s="3"/>
       <c r="H30" s="4"/>
       <c r="I30" s="4"/>
       <c r="J30" s="4"/>
@@ -1677,23 +1660,23 @@
       <c r="AC30" s="4"/>
     </row>
     <row r="31">
-      <c r="A31" s="12"/>
-      <c r="B31" s="7" t="s">
+      <c r="A31" s="5"/>
+      <c r="B31" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C31" s="7" t="s">
+      <c r="C31" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D31" s="7" t="s">
+      <c r="D31" s="6" t="s">
         <v>7</v>
       </c>
       <c r="E31" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="F31" s="7" t="s">
+      <c r="F31" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="G31" s="11"/>
+      <c r="G31" s="3"/>
       <c r="H31" s="4"/>
       <c r="I31" s="4"/>
       <c r="J31" s="4"/>
@@ -1718,13 +1701,13 @@
       <c r="AC31" s="4"/>
     </row>
     <row r="32">
-      <c r="A32" s="12"/>
-      <c r="B32" s="12"/>
-      <c r="C32" s="12"/>
-      <c r="D32" s="12"/>
-      <c r="E32" s="12"/>
-      <c r="F32" s="12"/>
-      <c r="G32" s="10" t="s">
+      <c r="A32" s="5"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="1" t="s">
         <v>38</v>
       </c>
       <c r="H32" s="4"/>
@@ -1751,7 +1734,7 @@
       <c r="AC32" s="4"/>
     </row>
     <row r="33">
-      <c r="A33" s="10" t="s">
+      <c r="A33" s="1" t="s">
         <v>43</v>
       </c>
       <c r="B33" s="2" t="s">
@@ -1769,7 +1752,7 @@
       <c r="F33" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G33" s="11"/>
+      <c r="G33" s="3"/>
       <c r="H33" s="4"/>
       <c r="I33" s="4"/>
       <c r="J33" s="4"/>
@@ -1794,23 +1777,23 @@
       <c r="AC33" s="4"/>
     </row>
     <row r="34">
-      <c r="A34" s="12"/>
-      <c r="B34" s="7" t="s">
+      <c r="A34" s="5"/>
+      <c r="B34" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C34" s="7" t="s">
+      <c r="C34" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D34" s="7" t="s">
+      <c r="D34" s="6" t="s">
         <v>7</v>
       </c>
       <c r="E34" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="F34" s="7" t="s">
+      <c r="F34" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="G34" s="11"/>
+      <c r="G34" s="3"/>
       <c r="H34" s="4"/>
       <c r="I34" s="4"/>
       <c r="J34" s="4"/>
@@ -1835,13 +1818,13 @@
       <c r="AC34" s="4"/>
     </row>
     <row r="35">
-      <c r="A35" s="12"/>
-      <c r="B35" s="12"/>
-      <c r="C35" s="12"/>
-      <c r="D35" s="12"/>
-      <c r="E35" s="12"/>
-      <c r="F35" s="12"/>
-      <c r="G35" s="10" t="s">
+      <c r="A35" s="5"/>
+      <c r="B35" s="5"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="5"/>
+      <c r="G35" s="1" t="s">
         <v>43</v>
       </c>
       <c r="H35" s="4"/>

</xml_diff>